<commit_message>
classes of different category created
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ubisoft\Courses\Projects\Billing Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3650DC20-E598-4A11-B18A-F3AE8B39DFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB98C9A-6119-45E2-B23F-A6342216CB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies CD" sheetId="2" r:id="rId1"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C1A00B-9A1B-4F49-8553-6287DA8B8AE4}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +698,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFF03A4-021D-4791-BFF4-0627F9661AC3}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
stage 2: problem of double quantity is solved
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ubisoft\Courses\Projects\Billing Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386CB224-6550-4164-A8B0-2426208515EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06CC6BA-1AAE-4F7D-805E-BE58862F5C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1121,7 +1121,7 @@
         <v>6000</v>
       </c>
       <c r="D5" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1135,7 +1135,7 @@
         <v>2500</v>
       </c>
       <c r="D6" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
discount calculation is complete
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ubisoft\Courses\Projects\Billing Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06CC6BA-1AAE-4F7D-805E-BE58862F5C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9512B6-3A6F-44DC-9739-00AFCFE7D334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movies CD" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Fruits" sheetId="3" r:id="rId3"/>
     <sheet name="Games" sheetId="5" r:id="rId4"/>
     <sheet name="Sports Kit" sheetId="6" r:id="rId5"/>
+    <sheet name="Discount" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -191,6 +192,12 @@
   </si>
   <si>
     <t>Hockey</t>
+  </si>
+  <si>
+    <t>Today's Discount</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -760,7 +767,7 @@
         <v>320</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1217,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA33D2AB-F332-422B-96BE-9AD795C2F9D9}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1279,7 +1286,7 @@
         <v>5000</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1378,6 +1385,35 @@
       </c>
       <c r="D11" s="1">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850F152C-CD68-4093-8D75-D60894397C6A}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mutex added t prevent from multiple instance running
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ubisoft\Courses\Projects\Billing Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5A40C9-4838-454D-BD23-94121FB15A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811568F2-56E9-418A-A270-26311C6F89D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -809,7 +809,7 @@
         <v>420</v>
       </c>
       <c r="D7" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1328,7 +1328,7 @@
         <v>6500</v>
       </c>
       <c r="D7" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
bill generated in file
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ubisoft\Courses\Projects\Billing Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811568F2-56E9-418A-A270-26311C6F89D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646DD926-D565-413B-96C4-7D5C946EF685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -767,7 +767,7 @@
         <v>320</v>
       </c>
       <c r="D4" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -823,7 +823,7 @@
         <v>100</v>
       </c>
       <c r="D8" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -865,7 +865,7 @@
         <v>180</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -955,7 +955,7 @@
         <v>80</v>
       </c>
       <c r="D5" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -969,7 +969,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>5000</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1212,7 +1212,7 @@
         <v>2000</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1258,7 @@
         <v>2000</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1356,7 +1356,7 @@
         <v>5999</v>
       </c>
       <c r="D9" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>